<commit_message>
added write feature for printing inventory to text file
</commit_message>
<xml_diff>
--- a/static/racquet_inventory.xlsx
+++ b/static/racquet_inventory.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hanxu/Documents/MSSD/CS 622/RacMatch_Project/static/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F1A3C89-548C-5F4C-9EDE-0DCC986B5731}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4AD9363B-49F8-274E-9D0D-99C990D651C8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5280" yWindow="2160" windowWidth="28040" windowHeight="17440" xr2:uid="{9934CBB0-134D-324D-8A2E-322FBBDDDE22}"/>
+    <workbookView xWindow="280" yWindow="460" windowWidth="22140" windowHeight="18400" xr2:uid="{9934CBB0-134D-324D-8A2E-322FBBDDDE22}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
   <si>
     <t>ID</t>
   </si>
@@ -78,15 +78,32 @@
     <t>STRENGTH</t>
   </si>
   <si>
-    <t>DESCRIPTION</t>
+    <t>Mizuno</t>
+  </si>
+  <si>
+    <t>Fortius 30 Power</t>
+  </si>
+  <si>
+    <t>Carlton</t>
+  </si>
+  <si>
+    <t>Air Edge</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -114,9 +131,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="1" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -431,52 +450,48 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C9F047E9-C48D-9F4D-A591-42DCC8655D06}">
-  <dimension ref="A1:J4"/>
+  <dimension ref="A1:I6"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="H5" sqref="H5"/>
+      <selection activeCell="J6" sqref="J6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="10.83203125" style="1"/>
     <col min="3" max="3" width="15" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="12.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F1" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="G1" t="s">
+      <c r="G1" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="H1" t="s">
+      <c r="H1" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="I1" t="s">
+      <c r="I1" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="J1" t="s">
-        <v>15</v>
-      </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -502,10 +517,10 @@
         <v>4</v>
       </c>
       <c r="I2">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3" s="1">
         <v>2</v>
       </c>
@@ -528,13 +543,13 @@
         <v>5</v>
       </c>
       <c r="H3">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="I3">
-        <v>8</v>
+        <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4" s="1">
         <v>3</v>
       </c>
@@ -560,10 +575,69 @@
         <v>5</v>
       </c>
       <c r="I4">
-        <v>4</v>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A5" s="1">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C5" t="s">
+        <v>16</v>
+      </c>
+      <c r="D5">
+        <v>4</v>
+      </c>
+      <c r="E5">
+        <v>9</v>
+      </c>
+      <c r="F5">
+        <v>9</v>
+      </c>
+      <c r="G5">
+        <v>5</v>
+      </c>
+      <c r="H5">
+        <v>5</v>
+      </c>
+      <c r="I5">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A6" s="1">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>17</v>
+      </c>
+      <c r="C6" t="s">
+        <v>18</v>
+      </c>
+      <c r="D6">
+        <v>3</v>
+      </c>
+      <c r="E6">
+        <v>4</v>
+      </c>
+      <c r="F6">
+        <v>6</v>
+      </c>
+      <c r="G6">
+        <v>2</v>
+      </c>
+      <c r="H6">
+        <v>3</v>
+      </c>
+      <c r="I6">
+        <v>2</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
tests for Inventory class
</commit_message>
<xml_diff>
--- a/static/racquet_inventory.xlsx
+++ b/static/racquet_inventory.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hanxu/Documents/MSSD/CS 622/RacMatch_Project/static/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4AD9363B-49F8-274E-9D0D-99C990D651C8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9304DB07-6617-7541-90A4-C23ABC9E477D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="280" yWindow="460" windowWidth="22140" windowHeight="18400" xr2:uid="{9934CBB0-134D-324D-8A2E-322FBBDDDE22}"/>
+    <workbookView xWindow="840" yWindow="460" windowWidth="19900" windowHeight="18400" xr2:uid="{9934CBB0-134D-324D-8A2E-322FBBDDDE22}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -131,11 +131,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="1" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -453,12 +454,12 @@
   <dimension ref="A1:I6"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="J6" sqref="J6"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="10.83203125" style="1"/>
+    <col min="1" max="1" width="7" style="1" customWidth="1"/>
     <col min="3" max="3" width="15" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -492,7 +493,7 @@
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A2" s="1">
+      <c r="A2" s="4">
         <v>1</v>
       </c>
       <c r="B2" t="s">

</xml_diff>

<commit_message>
validation for racquet field ranges from input file
</commit_message>
<xml_diff>
--- a/static/racquet_inventory.xlsx
+++ b/static/racquet_inventory.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hanxu/Documents/MSSD/CS 622/RacMatch_Project/static/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9304DB07-6617-7541-90A4-C23ABC9E477D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA68A68F-D01F-C14A-B3C2-E04AE6C3245B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="840" yWindow="460" windowWidth="19900" windowHeight="18400" xr2:uid="{9934CBB0-134D-324D-8A2E-322FBBDDDE22}"/>
+    <workbookView xWindow="21620" yWindow="460" windowWidth="19900" windowHeight="18400" xr2:uid="{9934CBB0-134D-324D-8A2E-322FBBDDDE22}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -454,7 +454,7 @@
   <dimension ref="A1:I6"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -532,7 +532,7 @@
         <v>6</v>
       </c>
       <c r="D3">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="E3">
         <v>7</v>

</xml_diff>

<commit_message>
minor changes in refactoring to generics
</commit_message>
<xml_diff>
--- a/static/racquet_inventory.xlsx
+++ b/static/racquet_inventory.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hanxu/Documents/MSSD/CS 622/RacMatch_Project/static/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA68A68F-D01F-C14A-B3C2-E04AE6C3245B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C776F0AE-79B6-4C4A-90B8-6CE2876C59BF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="21620" yWindow="460" windowWidth="19900" windowHeight="18400" xr2:uid="{9934CBB0-134D-324D-8A2E-322FBBDDDE22}"/>
+    <workbookView xWindow="13360" yWindow="2540" windowWidth="19900" windowHeight="18400" xr2:uid="{9934CBB0-134D-324D-8A2E-322FBBDDDE22}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -454,7 +454,7 @@
   <dimension ref="A1:I6"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -506,7 +506,7 @@
         <v>3</v>
       </c>
       <c r="E2">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="F2">
         <v>8</v>

</xml_diff>

<commit_message>
calculating matchIndex tested successfully
</commit_message>
<xml_diff>
--- a/static/racquet_inventory.xlsx
+++ b/static/racquet_inventory.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hanxu/Documents/MSSD/CS 622/RacMatch_Project/static/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C776F0AE-79B6-4C4A-90B8-6CE2876C59BF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A50DB003-E679-834B-B74A-F774C6941F21}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="13360" yWindow="2540" windowWidth="19900" windowHeight="18400" xr2:uid="{9934CBB0-134D-324D-8A2E-322FBBDDDE22}"/>
+    <workbookView xWindow="12120" yWindow="2400" windowWidth="21380" windowHeight="18400" xr2:uid="{9934CBB0-134D-324D-8A2E-322FBBDDDE22}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
   <si>
     <t>ID</t>
   </si>
@@ -88,6 +88,9 @@
   </si>
   <si>
     <t>Air Edge</t>
+  </si>
+  <si>
+    <t>SHAFTDIAMETER</t>
   </si>
 </sst>
 </file>
@@ -451,10 +454,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C9F047E9-C48D-9F4D-A591-42DCC8655D06}">
-  <dimension ref="A1:I6"/>
+  <dimension ref="A1:J6"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+      <selection activeCell="J7" sqref="J7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -463,7 +466,7 @@
     <col min="3" max="3" width="15" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -491,8 +494,11 @@
       <c r="I1" s="3" t="s">
         <v>14</v>
       </c>
+      <c r="J1" s="3" t="s">
+        <v>19</v>
+      </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A2" s="4">
         <v>1</v>
       </c>
@@ -520,8 +526,11 @@
       <c r="I2">
         <v>3</v>
       </c>
+      <c r="J2">
+        <v>8.3000000000000007</v>
+      </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A3" s="1">
         <v>2</v>
       </c>
@@ -549,8 +558,11 @@
       <c r="I3">
         <v>4</v>
       </c>
+      <c r="J3">
+        <v>6.9</v>
+      </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A4" s="1">
         <v>3</v>
       </c>
@@ -578,8 +590,11 @@
       <c r="I4">
         <v>3</v>
       </c>
+      <c r="J4">
+        <v>7.5</v>
+      </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A5" s="1">
         <v>4</v>
       </c>
@@ -607,8 +622,11 @@
       <c r="I5">
         <v>5</v>
       </c>
+      <c r="J5">
+        <v>7.7</v>
+      </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A6" s="1">
         <v>5</v>
       </c>
@@ -635,6 +653,9 @@
       </c>
       <c r="I6">
         <v>2</v>
+      </c>
+      <c r="J6">
+        <v>7.3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
get all racquets from database
</commit_message>
<xml_diff>
--- a/static/racquet_inventory.xlsx
+++ b/static/racquet_inventory.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10113"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10209"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hanxu/Documents/MSSD/CS 622/RacMatch_Project/static/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hanxu/Documents/MSSD/CS 622/Matchr_Project/static/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A50DB003-E679-834B-B74A-F774C6941F21}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0CE49B27-B511-E84B-B9F2-3B096FAE1E4A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="12120" yWindow="2400" windowWidth="21380" windowHeight="18400" xr2:uid="{9934CBB0-134D-324D-8A2E-322FBBDDDE22}"/>
+    <workbookView xWindow="240" yWindow="980" windowWidth="21760" windowHeight="18400" xr2:uid="{9934CBB0-134D-324D-8A2E-322FBBDDDE22}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -97,6 +97,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="166" formatCode="0.0"/>
+  </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -134,12 +137,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="1" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -457,7 +461,7 @@
   <dimension ref="A1:J6"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="J7" sqref="J7"/>
+      <selection activeCell="I10" sqref="I10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -508,25 +512,25 @@
       <c r="C2" t="s">
         <v>4</v>
       </c>
-      <c r="D2">
-        <v>3</v>
-      </c>
-      <c r="E2">
-        <v>5</v>
-      </c>
-      <c r="F2">
+      <c r="D2" s="1">
+        <v>3</v>
+      </c>
+      <c r="E2" s="1">
+        <v>5</v>
+      </c>
+      <c r="F2" s="1">
         <v>8</v>
       </c>
-      <c r="G2">
-        <v>3</v>
-      </c>
-      <c r="H2">
+      <c r="G2" s="1">
+        <v>3</v>
+      </c>
+      <c r="H2" s="1">
         <v>4</v>
       </c>
-      <c r="I2">
-        <v>3</v>
-      </c>
-      <c r="J2">
+      <c r="I2" s="1">
+        <v>3</v>
+      </c>
+      <c r="J2" s="5">
         <v>8.3000000000000007</v>
       </c>
     </row>
@@ -540,25 +544,25 @@
       <c r="C3" t="s">
         <v>6</v>
       </c>
-      <c r="D3">
-        <v>5</v>
-      </c>
-      <c r="E3">
+      <c r="D3" s="1">
+        <v>5</v>
+      </c>
+      <c r="E3" s="1">
         <v>7</v>
       </c>
-      <c r="F3">
+      <c r="F3" s="1">
         <v>8</v>
       </c>
-      <c r="G3">
-        <v>5</v>
-      </c>
-      <c r="H3">
-        <v>3</v>
-      </c>
-      <c r="I3">
+      <c r="G3" s="1">
+        <v>5</v>
+      </c>
+      <c r="H3" s="1">
+        <v>3</v>
+      </c>
+      <c r="I3" s="1">
         <v>4</v>
       </c>
-      <c r="J3">
+      <c r="J3" s="5">
         <v>6.9</v>
       </c>
     </row>
@@ -572,25 +576,25 @@
       <c r="C4" t="s">
         <v>8</v>
       </c>
-      <c r="D4">
-        <v>3</v>
-      </c>
-      <c r="E4">
+      <c r="D4" s="1">
+        <v>3</v>
+      </c>
+      <c r="E4" s="1">
         <v>6</v>
       </c>
-      <c r="F4">
+      <c r="F4" s="1">
         <v>7</v>
       </c>
-      <c r="G4">
+      <c r="G4" s="1">
         <v>4</v>
       </c>
-      <c r="H4">
-        <v>5</v>
-      </c>
-      <c r="I4">
-        <v>3</v>
-      </c>
-      <c r="J4">
+      <c r="H4" s="1">
+        <v>5</v>
+      </c>
+      <c r="I4" s="1">
+        <v>3</v>
+      </c>
+      <c r="J4" s="5">
         <v>7.5</v>
       </c>
     </row>
@@ -604,25 +608,25 @@
       <c r="C5" t="s">
         <v>16</v>
       </c>
-      <c r="D5">
+      <c r="D5" s="1">
         <v>4</v>
       </c>
-      <c r="E5">
+      <c r="E5" s="1">
         <v>9</v>
       </c>
-      <c r="F5">
+      <c r="F5" s="1">
         <v>9</v>
       </c>
-      <c r="G5">
-        <v>5</v>
-      </c>
-      <c r="H5">
-        <v>5</v>
-      </c>
-      <c r="I5">
-        <v>5</v>
-      </c>
-      <c r="J5">
+      <c r="G5" s="1">
+        <v>5</v>
+      </c>
+      <c r="H5" s="1">
+        <v>5</v>
+      </c>
+      <c r="I5" s="1">
+        <v>5</v>
+      </c>
+      <c r="J5" s="5">
         <v>7.7</v>
       </c>
     </row>
@@ -636,25 +640,25 @@
       <c r="C6" t="s">
         <v>18</v>
       </c>
-      <c r="D6">
-        <v>3</v>
-      </c>
-      <c r="E6">
+      <c r="D6" s="1">
+        <v>3</v>
+      </c>
+      <c r="E6" s="1">
         <v>4</v>
       </c>
-      <c r="F6">
+      <c r="F6" s="1">
         <v>6</v>
       </c>
-      <c r="G6">
+      <c r="G6" s="1">
         <v>2</v>
       </c>
-      <c r="H6">
-        <v>3</v>
-      </c>
-      <c r="I6">
+      <c r="H6" s="1">
+        <v>3</v>
+      </c>
+      <c r="I6" s="1">
         <v>2</v>
       </c>
-      <c r="J6">
+      <c r="J6" s="5">
         <v>7.3</v>
       </c>
     </row>

</xml_diff>